<commit_message>
add hgt data from tinysoft
</commit_message>
<xml_diff>
--- a/FactorLib/resource/tsl_tableinfo.xlsx
+++ b/FactorLib/resource/tsl_tableinfo.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{4CDDE27A-73FF-47D7-BC19-AB512B357D39}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA355805-8DBC-464F-9680-B52564CE0DDE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FactorID" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -199,6 +199,30 @@
   </si>
   <si>
     <t>note</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>截止日</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>股数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shares_hold</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>占总股本比例(%)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ratio_hold</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -536,20 +560,20 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.375" customWidth="1"/>
-    <col min="3" max="3" width="36.25" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -563,7 +587,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -577,7 +601,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -591,7 +615,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -605,7 +629,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -619,7 +643,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -633,7 +657,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -647,7 +671,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -661,7 +685,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -675,7 +699,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -689,7 +713,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -703,7 +727,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -717,7 +741,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -731,7 +755,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -745,7 +769,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -759,7 +783,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -773,7 +797,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -787,7 +811,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -801,7 +825,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>28</v>
       </c>
@@ -815,7 +839,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -829,7 +853,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>30</v>
       </c>
@@ -843,7 +867,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>31</v>
       </c>
@@ -855,6 +879,48 @@
       </c>
       <c r="D22">
         <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23">
+        <v>132001</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D23">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24">
+        <v>132002</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D24">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25">
+        <v>132003</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D25">
+        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>